<commit_message>
All Lead Page updated
</commit_message>
<xml_diff>
--- a/PageObjectModelCucumber/src/main/java/org/testleaf/qa/testdata/LeadsFullData.xlsx
+++ b/PageObjectModelCucumber/src/main/java/org/testleaf/qa/testdata/LeadsFullData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mouneesh\eclipse-workspace\SeleniumTraining\PageObjectModel\src\main\java\org\testleaf\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mouneesh\git\repository4\PageObjectModelCucumber\src\main\java\org\testleaf\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD22A0-2903-4E54-8D66-D202DFADC7F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287A9147-B540-4A68-9046-814B48995DE7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FF41C036-37EB-4A4C-A936-DACDFFFD4641}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{FF41C036-37EB-4A4C-A936-DACDFFFD4641}"/>
   </bookViews>
   <sheets>
     <sheet name="Create_Lead" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>userName</t>
   </si>
@@ -113,6 +113,21 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>noredcords</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>duplicateTitleName</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Norecords</t>
   </si>
 </sst>
 </file>
@@ -503,7 +518,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27742AD9-3A18-4F5B-A095-E96D02CA7714}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,10 +670,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B637D14-647B-4CD2-86FF-083678DA0CEB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,9 +681,10 @@
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -678,8 +694,11 @@
       <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -689,8 +708,11 @@
       <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -699,6 +721,9 @@
       </c>
       <c r="C3" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -708,10 +733,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4A9CD2-CD5B-4BD0-9A51-B9BC9C4CE7B4}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,9 +744,10 @@
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -731,8 +757,11 @@
       <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -741,6 +770,9 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -750,10 +782,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878A4E88-3B2F-40FF-BC3F-8EC574A6EA37}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,9 +793,10 @@
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -776,8 +809,11 @@
       <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -789,6 +825,9 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>